<commit_message>
sửa lại quy tắt đáp án
</commit_message>
<xml_diff>
--- a/Data_Maker/Data_sheet_here/data_p1.xlsx
+++ b/Data_Maker/Data_sheet_here/data_p1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:BW7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,364 +436,2639 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Team1</t>
+          <t>Country1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Logo1</t>
+          <t>Audio1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Team2</t>
+          <t>Flag1</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Logo2</t>
+          <t>Country2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Team3</t>
+          <t>Audio2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Logo3</t>
+          <t>Flag2</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Team4</t>
+          <t>Country3</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Logo4</t>
+          <t>Audio3</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Team5</t>
+          <t>Flag3</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Logo5</t>
+          <t>Country4</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Audio4</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Flag4</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Country5</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Audio5</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Flag5</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Country6</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Audio6</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Flag6</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Country7</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Audio7</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Flag7</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Country8</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Audio8</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Flag8</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Country9</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Audio9</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Flag9</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>Country10</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Audio10</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Flag10</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Country11</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Audio11</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>Flag11</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>Country12</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>Audio12</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Flag12</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>Country13</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Audio13</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>Flag13</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>Country14</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>Audio14</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>Flag14</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>Country15</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>Audio15</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>Flag15</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>Country16</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>Audio16</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>Flag16</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>Country17</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>Audio17</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>Flag17</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>Country18</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>Audio18</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>Flag18</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>Country19</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>Audio19</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>Flag19</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>Country20</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>Audio20</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>Flag20</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>Country21</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>Audio21</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>Flag21</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>Country22</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>Audio22</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>Flag22</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>Country23</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>Audio23</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>Flag23</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>Country24</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>Audio24</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>Flag24</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>Country25</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>Audio25</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>Flag25</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Philadelphia Eagles.png</t>
+          <t>Morocco.mp3</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Green Bay Packers</t>
+          <t>ma.png</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Green Bay Packers.png</t>
+          <t>Nepal</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>New York Giants</t>
+          <t>Nepal.mp3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> New York Giants.png</t>
+          <t>np.png</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>New Orleans Saints</t>
+          <t>Malawi</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>New Orleans Saints.png</t>
+          <t>Malawi.mp3</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars</t>
+          <t>mw.png</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Jacksonville Jaguars.png</t>
+          <t>Angola</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Angola.mp3</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>ao.png</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Luxembourg</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Luxembourg.mp3</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>lu.png</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Cambodia</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Cambodia.mp3</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>kh.png</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Haiti</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Haiti.mp3</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>ht.png</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>Croatia</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Croatia.mp3</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>hr.png</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Rwanda</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>Rwanda.mp3</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>rw.png</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>Pakistan</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>Pakistan.mp3</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>pk.png</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Slovenia</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Slovenia.mp3</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>si.png</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>Burkina Faso</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>Burkina Faso.mp3</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>bf.png</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>Denmark</t>
+        </is>
+      </c>
+      <c r="AL2" t="inlineStr">
+        <is>
+          <t>Denmark.mp3</t>
+        </is>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>dk.png</t>
+        </is>
+      </c>
+      <c r="AN2" t="inlineStr">
+        <is>
+          <t>Eswatini</t>
+        </is>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>Eswatini.mp3</t>
+        </is>
+      </c>
+      <c r="AP2" t="inlineStr">
+        <is>
+          <t>sz.png</t>
+        </is>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>Tanzania</t>
+        </is>
+      </c>
+      <c r="AR2" t="inlineStr">
+        <is>
+          <t>Tanzania.mp3</t>
+        </is>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>tz.png</t>
+        </is>
+      </c>
+      <c r="AT2" t="inlineStr">
+        <is>
+          <t>Lithuania</t>
+        </is>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>Lithuania.mp3</t>
+        </is>
+      </c>
+      <c r="AV2" t="inlineStr">
+        <is>
+          <t>lt.png</t>
+        </is>
+      </c>
+      <c r="AW2" t="inlineStr">
+        <is>
+          <t>Myanmar (Burma)</t>
+        </is>
+      </c>
+      <c r="AX2" t="inlineStr">
+        <is>
+          <t>Myanmar (Burma).mp3</t>
+        </is>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>mm.png</t>
+        </is>
+      </c>
+      <c r="AZ2" t="inlineStr">
+        <is>
+          <t>Burundi</t>
+        </is>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>Burundi.mp3</t>
+        </is>
+      </c>
+      <c r="BB2" t="inlineStr">
+        <is>
+          <t>bi.png</t>
+        </is>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>Azerbaijan</t>
+        </is>
+      </c>
+      <c r="BD2" t="inlineStr">
+        <is>
+          <t>Azerbaijan.mp3</t>
+        </is>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>az.png</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>Belgium</t>
+        </is>
+      </c>
+      <c r="BG2" t="inlineStr">
+        <is>
+          <t>Belgium.mp3</t>
+        </is>
+      </c>
+      <c r="BH2" t="inlineStr">
+        <is>
+          <t>be.png</t>
+        </is>
+      </c>
+      <c r="BI2" t="inlineStr">
+        <is>
+          <t>Estonia</t>
+        </is>
+      </c>
+      <c r="BJ2" t="inlineStr">
+        <is>
+          <t>Estonia.mp3</t>
+        </is>
+      </c>
+      <c r="BK2" t="inlineStr">
+        <is>
+          <t>ee.png</t>
+        </is>
+      </c>
+      <c r="BL2" t="inlineStr">
+        <is>
+          <t>Jordan</t>
+        </is>
+      </c>
+      <c r="BM2" t="inlineStr">
+        <is>
+          <t>Jordan.mp3</t>
+        </is>
+      </c>
+      <c r="BN2" t="inlineStr">
+        <is>
+          <t>jo.png</t>
+        </is>
+      </c>
+      <c r="BO2" t="inlineStr">
+        <is>
+          <t>South Africa</t>
+        </is>
+      </c>
+      <c r="BP2" t="inlineStr">
+        <is>
+          <t>South Africa.mp3</t>
+        </is>
+      </c>
+      <c r="BQ2" t="inlineStr">
+        <is>
+          <t>za.png</t>
+        </is>
+      </c>
+      <c r="BR2" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="BS2" t="inlineStr">
+        <is>
+          <t>Australia.mp3</t>
+        </is>
+      </c>
+      <c r="BT2" t="inlineStr">
+        <is>
+          <t>au.png</t>
+        </is>
+      </c>
+      <c r="BU2" t="inlineStr">
+        <is>
+          <t>Cuba</t>
+        </is>
+      </c>
+      <c r="BV2" t="inlineStr">
+        <is>
+          <t>Cuba.mp3</t>
+        </is>
+      </c>
+      <c r="BW2" t="inlineStr">
+        <is>
+          <t>cu.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Indianapolis Colts</t>
+          <t>Tajikistan</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Indianapolis Colts.png</t>
+          <t>Tajikistan.mp3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Washington Commanders</t>
+          <t>tj.png</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Washington Commanders.png</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers</t>
+          <t>Tunisia.mp3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Pittsburgh Steelers.png</t>
+          <t>tn.png</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Atlanta Falcons</t>
+          <t>Ghana</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Atlanta Falcons.png</t>
+          <t>Ghana.mp3</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Seattle Seahawks</t>
+          <t>gh.png</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Seattle Seahawks.png</t>
+          <t>Bangladesh</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Bangladesh.mp3</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>bd.png</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Czech Republic</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Czech Republic.mp3</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>cz.png</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Kazakhstan</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Kazakhstan.mp3</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>kz.png</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Canada.mp3</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>ca.png</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>Greece</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Greece.mp3</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>gr.png</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Mauritius</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>Mauritius.mp3</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>mu.png</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>Norway.mp3</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>no.png</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>Hungary</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Hungary.mp3</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>hu.png</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>Germany.mp3</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>de.png</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>Fiji</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>Fiji.mp3</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>fj.png</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>Qatar</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>Qatar.mp3</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>qa.png</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>Laos</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>Laos.mp3</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>la.png</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>Spain</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>Spain.mp3</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>es.png</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>Chad</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>Chad.mp3</t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>td.png</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>Timor-Leste</t>
+        </is>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>Timor-Leste.mp3</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>tl.png</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>Papua New Guinea</t>
+        </is>
+      </c>
+      <c r="BD3" t="inlineStr">
+        <is>
+          <t>Papua New Guinea.mp3</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>pg.png</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>Oman</t>
+        </is>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>Oman.mp3</t>
+        </is>
+      </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>om.png</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>North Macedonia</t>
+        </is>
+      </c>
+      <c r="BJ3" t="inlineStr">
+        <is>
+          <t>North Macedonia.mp3</t>
+        </is>
+      </c>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>mk.png</t>
+        </is>
+      </c>
+      <c r="BL3" t="inlineStr">
+        <is>
+          <t>Panama</t>
+        </is>
+      </c>
+      <c r="BM3" t="inlineStr">
+        <is>
+          <t>Panama.mp3</t>
+        </is>
+      </c>
+      <c r="BN3" t="inlineStr">
+        <is>
+          <t>pa.png</t>
+        </is>
+      </c>
+      <c r="BO3" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="BP3" t="inlineStr">
+        <is>
+          <t>France.mp3</t>
+        </is>
+      </c>
+      <c r="BQ3" t="inlineStr">
+        <is>
+          <t>fr.png</t>
+        </is>
+      </c>
+      <c r="BR3" t="inlineStr">
+        <is>
+          <t>Senegal</t>
+        </is>
+      </c>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>Senegal.mp3</t>
+        </is>
+      </c>
+      <c r="BT3" t="inlineStr">
+        <is>
+          <t>sn.png</t>
+        </is>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
+          <t>Venezuela</t>
+        </is>
+      </c>
+      <c r="BV3" t="inlineStr">
+        <is>
+          <t>Venezuela.mp3</t>
+        </is>
+      </c>
+      <c r="BW3" t="inlineStr">
+        <is>
+          <t>ve.png</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Minnesota Vikings</t>
+          <t>Kyrgyzstan</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Minnesota Vikings.png</t>
+          <t>Kyrgyzstan.mp3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Arizona Cardinals</t>
+          <t>kg.png</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Arizona Cardinals.png</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders</t>
+          <t>Slovakia.mp3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Las Vegas Raiders.png</t>
+          <t>sk.png</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>San Francisco 49ers</t>
+          <t>Armenia</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>San Francisco 49ers.png</t>
+          <t>Armenia.mp3</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Baltimore Ravens</t>
+          <t>am.png</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Baltimore Ravens.png</t>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Mexico.mp3</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>mx.png</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Sri Lanka</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Sri Lanka.mp3</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>lk.png</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Taiwan.mp3</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>tw.png</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>Israel</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Israel.mp3</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>il.png</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Iran</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Iran.mp3</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>ir.png</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Peru</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>Peru.mp3</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>pe.png</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Benin</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>Benin.mp3</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>bj.png</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>Albania</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Albania.mp3</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>al.png</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>Madagascar</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>Madagascar.mp3</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>mg.png</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>Kenya</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>Kenya.mp3</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>ke.png</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>Zimbabwe</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>Zimbabwe.mp3</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>zw.png</t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>Poland</t>
+        </is>
+      </c>
+      <c r="AR4" t="inlineStr">
+        <is>
+          <t>Poland.mp3</t>
+        </is>
+      </c>
+      <c r="AS4" t="inlineStr">
+        <is>
+          <t>pl.png</t>
+        </is>
+      </c>
+      <c r="AT4" t="inlineStr">
+        <is>
+          <t>Singapore</t>
+        </is>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>Singapore.mp3</t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>sg.png</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>Lebanon</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>Lebanon.mp3</t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>lb.png</t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr">
+        <is>
+          <t>Philippines</t>
+        </is>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>Philippines.mp3</t>
+        </is>
+      </c>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>ph.png</t>
+        </is>
+      </c>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>Afghanistan</t>
+        </is>
+      </c>
+      <c r="BD4" t="inlineStr">
+        <is>
+          <t>Afghanistan.mp3</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>af.png</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>Brazil</t>
+        </is>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>Brazil.mp3</t>
+        </is>
+      </c>
+      <c r="BH4" t="inlineStr">
+        <is>
+          <t>br.png</t>
+        </is>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>Niger</t>
+        </is>
+      </c>
+      <c r="BJ4" t="inlineStr">
+        <is>
+          <t>Niger.mp3</t>
+        </is>
+      </c>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>ne.png</t>
+        </is>
+      </c>
+      <c r="BL4" t="inlineStr">
+        <is>
+          <t>Austria</t>
+        </is>
+      </c>
+      <c r="BM4" t="inlineStr">
+        <is>
+          <t>Austria.mp3</t>
+        </is>
+      </c>
+      <c r="BN4" t="inlineStr">
+        <is>
+          <t>at.png</t>
+        </is>
+      </c>
+      <c r="BO4" t="inlineStr">
+        <is>
+          <t>Egypt</t>
+        </is>
+      </c>
+      <c r="BP4" t="inlineStr">
+        <is>
+          <t>Egypt.mp3</t>
+        </is>
+      </c>
+      <c r="BQ4" t="inlineStr">
+        <is>
+          <t>eg.png</t>
+        </is>
+      </c>
+      <c r="BR4" t="inlineStr">
+        <is>
+          <t>Nigeria</t>
+        </is>
+      </c>
+      <c r="BS4" t="inlineStr">
+        <is>
+          <t>Nigeria.mp3</t>
+        </is>
+      </c>
+      <c r="BT4" t="inlineStr">
+        <is>
+          <t>ng.png</t>
+        </is>
+      </c>
+      <c r="BU4" t="inlineStr">
+        <is>
+          <t>Latvia</t>
+        </is>
+      </c>
+      <c r="BV4" t="inlineStr">
+        <is>
+          <t>Latvia.mp3</t>
+        </is>
+      </c>
+      <c r="BW4" t="inlineStr">
+        <is>
+          <t>lv.png</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Denver Broncos</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Denver Broncos.png</t>
+          <t>Colombia.mp3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers</t>
+          <t>co.png</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Tampa Bay Buccaneers.png</t>
+          <t>Mali</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dallas Cowboys</t>
+          <t>Mali.mp3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dallas Cowboys.png</t>
+          <t>ml.png</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Los Angeles Rams</t>
+          <t>Barbados</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Los Angeles Rams.png</t>
+          <t>Barbados.mp3</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Buffalo Bills</t>
+          <t>bb.png</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Buffalo Bills.png</t>
+          <t>New Zealand</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>New Zealand.mp3</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>nz.png</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Algeria</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Algeria.mp3</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>dz.png</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Trinidad and Tobago.mp3</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>tt.png</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>Bulgaria</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Bulgaria.mp3</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>bg.png</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>Honduras</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Honduras.mp3</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>hn.png</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Antigua and Barbuda</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>Antigua and Barbuda.mp3</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>ag.png</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>Jamaica</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Jamaica.mp3</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>jm.png</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>Sudan</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Sudan.mp3</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>sd.png</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>Chile</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>Chile.mp3</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>cl.png</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>Mozambique</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>Mozambique.mp3</t>
+        </is>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t>mz.png</t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>Sierra Leone</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>Sierra Leone.mp3</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>sl.png</t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="AR5" t="inlineStr">
+        <is>
+          <t>Italy.mp3</t>
+        </is>
+      </c>
+      <c r="AS5" t="inlineStr">
+        <is>
+          <t>it.png</t>
+        </is>
+      </c>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t>Costa Rica</t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>Costa Rica.mp3</t>
+        </is>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>cr.png</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>India.mp3</t>
+        </is>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>in.png</t>
+        </is>
+      </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t>Ecuador</t>
+        </is>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>Ecuador.mp3</t>
+        </is>
+      </c>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>ec.png</t>
+        </is>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>Uganda</t>
+        </is>
+      </c>
+      <c r="BD5" t="inlineStr">
+        <is>
+          <t>Uganda.mp3</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>ug.png</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>Guatemala</t>
+        </is>
+      </c>
+      <c r="BG5" t="inlineStr">
+        <is>
+          <t>Guatemala.mp3</t>
+        </is>
+      </c>
+      <c r="BH5" t="inlineStr">
+        <is>
+          <t>gt.png</t>
+        </is>
+      </c>
+      <c r="BI5" t="inlineStr">
+        <is>
+          <t>Paraguay</t>
+        </is>
+      </c>
+      <c r="BJ5" t="inlineStr">
+        <is>
+          <t>Paraguay.mp3</t>
+        </is>
+      </c>
+      <c r="BK5" t="inlineStr">
+        <is>
+          <t>py.png</t>
+        </is>
+      </c>
+      <c r="BL5" t="inlineStr">
+        <is>
+          <t>Lesotho</t>
+        </is>
+      </c>
+      <c r="BM5" t="inlineStr">
+        <is>
+          <t>Lesotho.mp3</t>
+        </is>
+      </c>
+      <c r="BN5" t="inlineStr">
+        <is>
+          <t>ls.png</t>
+        </is>
+      </c>
+      <c r="BO5" t="inlineStr">
+        <is>
+          <t>Liberia</t>
+        </is>
+      </c>
+      <c r="BP5" t="inlineStr">
+        <is>
+          <t>Liberia.mp3</t>
+        </is>
+      </c>
+      <c r="BQ5" t="inlineStr">
+        <is>
+          <t>lr.png</t>
+        </is>
+      </c>
+      <c r="BR5" t="inlineStr">
+        <is>
+          <t>Somalia</t>
+        </is>
+      </c>
+      <c r="BS5" t="inlineStr">
+        <is>
+          <t>Somalia.mp3</t>
+        </is>
+      </c>
+      <c r="BT5" t="inlineStr">
+        <is>
+          <t>so.png</t>
+        </is>
+      </c>
+      <c r="BU5" t="inlineStr">
+        <is>
+          <t>Montenegro</t>
+        </is>
+      </c>
+      <c r="BV5" t="inlineStr">
+        <is>
+          <t>Montenegro.mp3</t>
+        </is>
+      </c>
+      <c r="BW5" t="inlineStr">
+        <is>
+          <t>me.png</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>New England Patriots</t>
+          <t>Ethiopia</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>New England Patriots.png</t>
+          <t>Ethiopia.mp3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Tennessee Titans</t>
+          <t>et.png</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Tennessee Titans.png</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Carolina Panthers</t>
+          <t>Sweden.mp3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Carolina Panthers.png</t>
+          <t>se.png</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Cincinnati Bengals.png</t>
+          <t>Romania.mp3</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Detroit Lions</t>
+          <t>ro.png</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Detroit Lions.png</t>
+          <t>Ireland</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Ireland.mp3</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>ie.png</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Bahamas</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Bahamas.mp3</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>bs.png</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Indonesia</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Indonesia.mp3</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>id.png</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Monaco</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Monaco.mp3</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>mc.png</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>United States.mp3</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>us.png</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>Netherlands.mp3</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>nl.png</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>Djibouti</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>Djibouti.mp3</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>dj.png</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Russia.mp3</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>ru.png</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>Serbia</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>Serbia.mp3</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>rs.png</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>Belize</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>Belize.mp3</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>bz.png</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>Cameroon</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>Cameroon.mp3</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>cm.png</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>El Salvador</t>
+        </is>
+      </c>
+      <c r="AR6" t="inlineStr">
+        <is>
+          <t>El Salvador.mp3</t>
+        </is>
+      </c>
+      <c r="AS6" t="inlineStr">
+        <is>
+          <t>sv.png</t>
+        </is>
+      </c>
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t>Zambia</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>Zambia.mp3</t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>zm.png</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>Cyprus</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>Cyprus.mp3</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>cy.png</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>Moldova</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>Moldova.mp3</t>
+        </is>
+      </c>
+      <c r="BB6" t="inlineStr">
+        <is>
+          <t>md.png</t>
+        </is>
+      </c>
+      <c r="BC6" t="inlineStr">
+        <is>
+          <t>Dominica</t>
+        </is>
+      </c>
+      <c r="BD6" t="inlineStr">
+        <is>
+          <t>Dominica.mp3</t>
+        </is>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>dm.png</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>Bahrain</t>
+        </is>
+      </c>
+      <c r="BG6" t="inlineStr">
+        <is>
+          <t>Bahrain.mp3</t>
+        </is>
+      </c>
+      <c r="BH6" t="inlineStr">
+        <is>
+          <t>bh.png</t>
+        </is>
+      </c>
+      <c r="BI6" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="BJ6" t="inlineStr">
+        <is>
+          <t>Thailand.mp3</t>
+        </is>
+      </c>
+      <c r="BK6" t="inlineStr">
+        <is>
+          <t>th.png</t>
+        </is>
+      </c>
+      <c r="BL6" t="inlineStr">
+        <is>
+          <t>Malaysia</t>
+        </is>
+      </c>
+      <c r="BM6" t="inlineStr">
+        <is>
+          <t>Malaysia.mp3</t>
+        </is>
+      </c>
+      <c r="BN6" t="inlineStr">
+        <is>
+          <t>my.png</t>
+        </is>
+      </c>
+      <c r="BO6" t="inlineStr">
+        <is>
+          <t>Bosnia and Herzegovina</t>
+        </is>
+      </c>
+      <c r="BP6" t="inlineStr">
+        <is>
+          <t>Bosnia and Herzegovina.mp3</t>
+        </is>
+      </c>
+      <c r="BQ6" t="inlineStr">
+        <is>
+          <t>ba.png</t>
+        </is>
+      </c>
+      <c r="BR6" t="inlineStr">
+        <is>
+          <t>Finland</t>
+        </is>
+      </c>
+      <c r="BS6" t="inlineStr">
+        <is>
+          <t>Finland.mp3</t>
+        </is>
+      </c>
+      <c r="BT6" t="inlineStr">
+        <is>
+          <t>fi.png</t>
+        </is>
+      </c>
+      <c r="BU6" t="inlineStr">
+        <is>
+          <t>Botswana</t>
+        </is>
+      </c>
+      <c r="BV6" t="inlineStr">
+        <is>
+          <t>Botswana.mp3</t>
+        </is>
+      </c>
+      <c r="BW6" t="inlineStr">
+        <is>
+          <t>bw.png</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chicago Bears</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Chicago Bears.png</t>
+          <t>Japan.mp3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cleveland Browns</t>
+          <t>jp.png</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Cleveland Browns.png</t>
+          <t>Bhutan</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers</t>
+          <t>Bhutan.mp3</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Los Angeles Chargers.png</t>
+          <t>bt.png</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Houston Texans</t>
+          <t>Belarus</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Houston Texans.png</t>
+          <t>Belarus.mp3</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>New York Jets</t>
+          <t>by.png</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>New York Jets.png</t>
+          <t>Turkey</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Turkey.mp3</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>tr.png</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Uzbekistan</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Uzbekistan.mp3</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>uz.png</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Portugal</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Portugal.mp3</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>pt.png</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Malta</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Malta.mp3</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>mt.png</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>China.mp3</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>cn.png</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>Ukraine</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>Ukraine.mp3</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>ua.png</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>South Korea</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>South Korea.mp3</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>kr.png</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>Kuwait</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>Kuwait.mp3</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>kw.png</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>Gabon</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>Gabon.mp3</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>ga.png</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>Saudi Arabia</t>
+        </is>
+      </c>
+      <c r="AL7" t="inlineStr">
+        <is>
+          <t>Saudi Arabia.mp3</t>
+        </is>
+      </c>
+      <c r="AM7" t="inlineStr">
+        <is>
+          <t>sa.png</t>
+        </is>
+      </c>
+      <c r="AN7" t="inlineStr">
+        <is>
+          <t>Iceland</t>
+        </is>
+      </c>
+      <c r="AO7" t="inlineStr">
+        <is>
+          <t>Iceland.mp3</t>
+        </is>
+      </c>
+      <c r="AP7" t="inlineStr">
+        <is>
+          <t>is.png</t>
+        </is>
+      </c>
+      <c r="AQ7" t="inlineStr">
+        <is>
+          <t>Dominican Republic</t>
+        </is>
+      </c>
+      <c r="AR7" t="inlineStr">
+        <is>
+          <t>Dominican Republic.mp3</t>
+        </is>
+      </c>
+      <c r="AS7" t="inlineStr">
+        <is>
+          <t>do.png</t>
+        </is>
+      </c>
+      <c r="AT7" t="inlineStr">
+        <is>
+          <t>Namibia</t>
+        </is>
+      </c>
+      <c r="AU7" t="inlineStr">
+        <is>
+          <t>Namibia.mp3</t>
+        </is>
+      </c>
+      <c r="AV7" t="inlineStr">
+        <is>
+          <t>na.png</t>
+        </is>
+      </c>
+      <c r="AW7" t="inlineStr">
+        <is>
+          <t>North Korea</t>
+        </is>
+      </c>
+      <c r="AX7" t="inlineStr">
+        <is>
+          <t>North Korea.mp3</t>
+        </is>
+      </c>
+      <c r="AY7" t="inlineStr">
+        <is>
+          <t>kp.png</t>
+        </is>
+      </c>
+      <c r="AZ7" t="inlineStr">
+        <is>
+          <t>Syria</t>
+        </is>
+      </c>
+      <c r="BA7" t="inlineStr">
+        <is>
+          <t>Syria.mp3</t>
+        </is>
+      </c>
+      <c r="BB7" t="inlineStr">
+        <is>
+          <t>sy.png</t>
+        </is>
+      </c>
+      <c r="BC7" t="inlineStr">
+        <is>
+          <t>United Arab Emirates</t>
+        </is>
+      </c>
+      <c r="BD7" t="inlineStr">
+        <is>
+          <t>United Arab Emirates.mp3</t>
+        </is>
+      </c>
+      <c r="BE7" t="inlineStr">
+        <is>
+          <t>ae.png</t>
+        </is>
+      </c>
+      <c r="BF7" t="inlineStr">
+        <is>
+          <t>Suriname</t>
+        </is>
+      </c>
+      <c r="BG7" t="inlineStr">
+        <is>
+          <t>Suriname.mp3</t>
+        </is>
+      </c>
+      <c r="BH7" t="inlineStr">
+        <is>
+          <t>sr.png</t>
+        </is>
+      </c>
+      <c r="BI7" t="inlineStr">
+        <is>
+          <t>Uruguay</t>
+        </is>
+      </c>
+      <c r="BJ7" t="inlineStr">
+        <is>
+          <t>Uruguay.mp3</t>
+        </is>
+      </c>
+      <c r="BK7" t="inlineStr">
+        <is>
+          <t>uy.png</t>
+        </is>
+      </c>
+      <c r="BL7" t="inlineStr">
+        <is>
+          <t>Turkmenistan</t>
+        </is>
+      </c>
+      <c r="BM7" t="inlineStr">
+        <is>
+          <t>Turkmenistan.mp3</t>
+        </is>
+      </c>
+      <c r="BN7" t="inlineStr">
+        <is>
+          <t>tm.png</t>
+        </is>
+      </c>
+      <c r="BO7" t="inlineStr">
+        <is>
+          <t>Iraq</t>
+        </is>
+      </c>
+      <c r="BP7" t="inlineStr">
+        <is>
+          <t>Iraq.mp3</t>
+        </is>
+      </c>
+      <c r="BQ7" t="inlineStr">
+        <is>
+          <t>iq.png</t>
+        </is>
+      </c>
+      <c r="BR7" t="inlineStr">
+        <is>
+          <t>Vietnam</t>
+        </is>
+      </c>
+      <c r="BS7" t="inlineStr">
+        <is>
+          <t>Vietnam.mp3</t>
+        </is>
+      </c>
+      <c r="BT7" t="inlineStr">
+        <is>
+          <t>vn.png</t>
+        </is>
+      </c>
+      <c r="BU7" t="inlineStr">
+        <is>
+          <t>South Sudan</t>
+        </is>
+      </c>
+      <c r="BV7" t="inlineStr">
+        <is>
+          <t>South Sudan.mp3</t>
+        </is>
+      </c>
+      <c r="BW7" t="inlineStr">
+        <is>
+          <t>ss.png</t>
         </is>
       </c>
     </row>

</xml_diff>